<commit_message>
Push - Updated Main with arguments and PDF variable
</commit_message>
<xml_diff>
--- a/Sales_Order_Entry_Robot_ChrisSanderson_RossMarshall/allOtherData.xlsx
+++ b/Sales_Order_Entry_Robot_ChrisSanderson_RossMarshall/allOtherData.xlsx
@@ -14,65 +14,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
-  <x:si>
-    <x:t>Column1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice Due</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <x:si>
+    <x:t>Company Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company Town</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company State</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company Contact</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company TIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company PIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer Town</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer State</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer PIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer TIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer Contact</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice Number</x:t>
   </x:si>
   <x:si>
     <x:t>Invoice Date</x:t>
   </x:si>
   <x:si>
+    <x:t>Due Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sub Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GST 8%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>J.K. Computers</x:t>
+  </x:si>
+  <x:si>
     <x:t>1133 South Cavalier Drive</x:t>
   </x:si>
   <x:si>
@@ -112,22 +118,22 @@
     <x:t>+3435677789</x:t>
   </x:si>
   <x:si>
-    <x:t>100</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10800.00</x:t>
+    <x:t xml:space="preserve"> 100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feb 23- 2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mar 10- 2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> 10800.00</x:t>
   </x:si>
   <x:si>
     <x:t>864.00</x:t>
   </x:si>
   <x:si>
-    <x:t>11664.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mar 10  2016</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Feb 23  2016</x:t>
+    <x:t xml:space="preserve">11664.00 </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -484,7 +490,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:19">
+    <x:row r="1" spans="1:20">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -542,64 +548,70 @@
       <x:c r="S1" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
+      <x:c r="T1" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:19">
+    <x:row r="2" spans="1:20">
       <x:c r="A2" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L2" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="N2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="P2" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>39</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>